<commit_message>
Added more to Run Predictions
</commit_message>
<xml_diff>
--- a/run_predictions/running_excel.xlsx
+++ b/run_predictions/running_excel.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -49,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -70,6 +71,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,7 +116,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -132,6 +134,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -152,13 +166,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.42"/>
@@ -181,72 +195,114 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>44914</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>0.0144097222222222</v>
+      <c r="A2" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>44917</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>0.0162152777777778</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>44913</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>0.0209722222222222</v>
+      <c r="A3" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>44916</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>0.0250347222222222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>44906</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>0.0329166666666667</v>
+      <c r="A4" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>44915</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>0.0380902777777778</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>44914</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0.0144097222222222</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>44913</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0.0209722222222222</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0.0329166666666667</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B8" s="1" t="n">
         <v>44901</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C8" s="2" t="n">
         <v>2.4</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D8" s="3" t="n">
         <v>0.0145138888888889</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B1005" type="date">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:B1008" type="date">
       <formula1>43831</formula1>
       <formula2>47847</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C1005" type="decimal">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C5:C1008" type="decimal">
       <formula1>0.1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D1005" type="time">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D1008" type="time">
       <formula1>0.0000115740740740741</formula1>
       <formula2>6.29165509259259</formula2>
     </dataValidation>

</xml_diff>